<commit_message>
Funcional (aunque desmodalurizada) version del programa
</commit_message>
<xml_diff>
--- a/values.xlsx
+++ b/values.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Juan</t>
   </si>
@@ -41,18 +41,29 @@
     <t>Lia</t>
   </si>
   <si>
-    <t>dgdgh</t>
-  </si>
-  <si>
-    <t>sss</t>
+    <t>Ramon</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Marcos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,9 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D1:E6"/>
+  <dimension ref="D1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -375,45 +388,56 @@
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+    <row r="9" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>